<commit_message>
ajout de nouvelle fonctionnabilité
</commit_message>
<xml_diff>
--- a/Document/estimation projet.xlsx
+++ b/Document/estimation projet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Semaine 15</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Le projet doit être décomposé en plusieurs sections indépendantes qui doivent être priorisées et estimées</t>
   </si>
   <si>
@@ -170,7 +167,22 @@
     <t>Reussir le gyroscope sur un projet test</t>
   </si>
   <si>
-    <t>Faire marcher le gyroscope sur le prjet principal en reglant le probleme de background</t>
+    <t>Faire marcher le gyroscope sur le projet principal en reglant le probleme de background</t>
+  </si>
+  <si>
+    <t>Finir le mouvement de la boule et mettre un son sur le bouton quitter pour essayer</t>
+  </si>
+  <si>
+    <t>Faire une bordure et avoir travailler sur le AsyncTask</t>
+  </si>
+  <si>
+    <t>Travailler sur AsyncTask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optimiser la vitesse de la boule,bouton quitter opérationnel,boule depasse pas les </t>
+  </si>
+  <si>
+    <t>bordures presque fini.</t>
   </si>
 </sst>
 </file>
@@ -352,6 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -367,7 +380,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1637,7 +1649,7 @@
   <sheetData>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1652,12 +1664,12 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1682,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="3">
         <v>25</v>
@@ -1693,7 +1705,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3">
         <v>25</v>
@@ -1704,7 +1716,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="3">
         <v>5</v>
@@ -1725,10 +1737,10 @@
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="20"/>
+      <c r="B21" s="21"/>
       <c r="C21" s="11">
         <f>SUM(C16:C20)</f>
         <v>55</v>
@@ -1762,7 +1774,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C26" s="3">
         <v>10</v>
@@ -1773,7 +1785,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C27" s="3">
         <v>10</v>
@@ -1784,7 +1796,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="3">
         <v>15</v>
@@ -1826,10 +1838,10 @@
       <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="20"/>
+      <c r="B34" s="21"/>
       <c r="C34" s="11">
         <f>SUM(C26:C33)</f>
         <v>35</v>
@@ -1856,8 +1868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1918,10 +1930,10 @@
         <v>43172</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1929,10 +1941,10 @@
         <v>43173</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1940,10 +1952,10 @@
         <v>43173</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1951,10 +1963,10 @@
         <v>43178</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1962,10 +1974,10 @@
         <v>43179</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1973,10 +1985,10 @@
         <v>43180</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1984,21 +1996,21 @@
         <v>43185</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="19">
+        <v>43186</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="24">
-        <v>43186</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>50</v>
-      </c>
       <c r="C21" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -2078,10 +2090,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="16">
         <f>SUM(C14:C21)</f>
         <v>0</v>
@@ -2089,13 +2101,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2104,24 +2116,24 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" s="21"/>
+        <v>29</v>
+      </c>
+      <c r="B42" s="22"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="22"/>
+      <c r="B43" s="23"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="22"/>
+      <c r="B44" s="23"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="22"/>
+      <c r="B46" s="23"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="23"/>
+      <c r="B47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2138,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2196,30 +2208,54 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12">
+        <v>43193</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="12">
+        <v>43195</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="12">
+        <v>43199</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="12">
+        <v>43200</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2313,10 +2349,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2324,13 +2360,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2339,24 +2375,24 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" s="21"/>
+        <v>29</v>
+      </c>
+      <c r="B42" s="22"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="22"/>
+      <c r="B43" s="23"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="22"/>
+      <c r="B44" s="23"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="22"/>
+      <c r="B46" s="23"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="23"/>
+      <c r="B47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2546,10 +2582,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2557,13 +2593,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2572,24 +2608,24 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" s="21"/>
+        <v>29</v>
+      </c>
+      <c r="B42" s="22"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="22"/>
+      <c r="B43" s="23"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="22"/>
+      <c r="B44" s="23"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="22"/>
+      <c r="B46" s="23"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="23"/>
+      <c r="B47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2643,7 +2679,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -2779,10 +2815,10 @@
       <c r="C36" s="15"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="20"/>
+      <c r="B37" s="21"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
         <v>0</v>
@@ -2790,13 +2826,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2805,24 +2841,24 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" s="21"/>
+        <v>29</v>
+      </c>
+      <c r="B42" s="22"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B43" s="22"/>
+      <c r="B43" s="23"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B44" s="22"/>
+      <c r="B44" s="23"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B45" s="22"/>
+      <c r="B45" s="23"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B46" s="22"/>
+      <c r="B46" s="23"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B47" s="23"/>
+      <c r="B47" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
rajout de projet et fin pour le projet
Arret du projet a cause du probleme avec le OnSensorChanged
</commit_message>
<xml_diff>
--- a/Document/estimation projet.xlsx
+++ b/Document/estimation projet.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -183,6 +183,24 @@
   </si>
   <si>
     <t>bordures presque fini.</t>
+  </si>
+  <si>
+    <t>Essayer de regler le probleme de la boule qui depasse et qui retourne sur la limite</t>
+  </si>
+  <si>
+    <t>3h30</t>
+  </si>
+  <si>
+    <t>Essayer de regler le probleme de la boule qui depasse et qui depasse pas</t>
+  </si>
+  <si>
+    <t>Regardez des exemples sur le onaccuracychanged</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Essayer de faire un score et regardez sur internet pour convertir les données de </t>
+  </si>
+  <si>
+    <t>l'accéléromètre</t>
   </si>
 </sst>
 </file>
@@ -2150,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2259,28 +2277,50 @@
       <c r="C18" s="15"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
+      <c r="A19" s="12">
+        <v>43201</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
+      <c r="A20" s="12">
+        <v>43206</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="C21" s="15"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="15"/>
+      <c r="A22" s="12">
+        <v>43208</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="C23" s="15"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Ajout de donnee mise a jour estimation
</commit_message>
<xml_diff>
--- a/Document/estimation projet.xlsx
+++ b/Document/estimation projet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="77">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -201,6 +201,54 @@
   </si>
   <si>
     <t>l'accéléromètre</t>
+  </si>
+  <si>
+    <t>Travailler pour bien faire marcher le gyroscope</t>
+  </si>
+  <si>
+    <t>Arrêt du projet de la boule</t>
+  </si>
+  <si>
+    <t>1h00</t>
+  </si>
+  <si>
+    <t>2h00</t>
+  </si>
+  <si>
+    <t>Debut projet de musique</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création d'image pause et play en paint </t>
+  </si>
+  <si>
+    <t>3h00</t>
+  </si>
+  <si>
+    <t>Faire marcher bouton play,pause et stop</t>
+  </si>
+  <si>
+    <t>Modifier code pour ajouter une autre musique et finir faire fonctionner le bouton stop</t>
+  </si>
+  <si>
+    <t>Faire marcher les boutons avancer,reculer,passer et avancer</t>
+  </si>
+  <si>
+    <t>Créer image avancer,reculer,passer et avancer.</t>
+  </si>
+  <si>
+    <t>4h00</t>
+  </si>
+  <si>
+    <t>Penser comment faire marcher la classe ajoutermusique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Penser a quoi rajouter,commencer créer un bouton ajouter musique.Tester des trucs </t>
+  </si>
+  <si>
+    <t>dans la classe</t>
   </si>
 </sst>
 </file>
@@ -1654,7 +1702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C36"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -1886,7 +1934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:F47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -2168,8 +2216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView view="pageLayout" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2449,8 +2497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView view="pageLayout" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2507,19 +2555,37 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12">
+        <v>43213</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="12">
+        <v>43214</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="12">
+        <v>43214</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
@@ -2527,38 +2593,74 @@
       <c r="C17" s="15"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
+      <c r="A18" s="12">
+        <v>43219</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
+      <c r="A19" s="12">
+        <v>43220</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
+      <c r="A20" s="12">
+        <v>43191</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
+      <c r="A21" s="12">
+        <v>43222</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="15"/>
+      <c r="B22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="15"/>
+      <c r="A23" s="12">
+        <v>43225</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -2682,8 +2784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2740,9 +2842,15 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12">
+        <v>43226</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>

</xml_diff>